<commit_message>
Added date for each ad.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\Programming\SoftUni\JS-SPA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="9408" windowWidth="23040" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -170,9 +165,6 @@
     <t>GitHub (up to 100)</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Basic Options (up to 130)</t>
   </si>
   <si>
@@ -201,9 +193,6 @@
   </si>
   <si>
     <t>https://github.com/ya-ivanov</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8</t>
   </si>
   <si>
     <t>yes</t>
@@ -237,46 +226,36 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="36">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="6">
@@ -312,70 +291,68 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalDown="1">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border diagonalDown="1">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border diagonalDown="1">
-      <left style="thin"/>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border diagonalDown="1">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border diagonalDown="1">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -405,6 +382,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,18 +404,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -701,29 +678,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="115" workbookViewId="0" tabSelected="1" zoomScaleNormal="115">
-      <selection pane="topLeft" activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="18" customHeight="1" r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
@@ -732,56 +710,56 @@
         <v>25</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row ht="18" customHeight="1" r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row ht="18" customHeight="1" r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="C5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -789,43 +767,43 @@
         <v>6</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row ht="18" customHeight="1" r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
@@ -837,7 +815,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
@@ -849,7 +827,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
@@ -861,7 +839,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -872,10 +850,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -887,7 +865,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
@@ -898,10 +876,10 @@
         <v>3</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
@@ -913,7 +891,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
@@ -925,7 +903,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
@@ -937,7 +915,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -949,7 +927,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
@@ -960,10 +938,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -975,7 +953,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
@@ -987,7 +965,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
@@ -998,10 +976,10 @@
         <v>5</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
@@ -1013,7 +991,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
@@ -1025,7 +1003,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
@@ -1037,7 +1015,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1049,7 +1027,7 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1039,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
@@ -1069,7 +1047,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -1081,225 +1059,225 @@
       </c>
       <c r="E32" s="5"/>
     </row>
-    <row ht="18" customHeight="1" r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row ht="18" customHeight="1" r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Error handling changes, other visual updates
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>∞</t>
   </si>
   <si>
     <t>https://github.com/ya-ivanov</t>
@@ -678,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,7 +686,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +723,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -736,7 +733,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -754,7 +751,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -764,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
+        <v>50</v>
+      </c>
+      <c r="D8" s="12">
         <v>6</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -776,10 +773,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>11</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="D9" s="12">
+        <v>13</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -796,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -850,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -876,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -938,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -976,7 +973,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
@@ -1084,7 +1081,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
@@ -1096,7 +1093,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
@@ -1108,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
@@ -1120,7 +1117,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
@@ -1132,7 +1129,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
@@ -1144,7 +1141,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
@@ -1156,7 +1153,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
@@ -1168,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
@@ -1180,7 +1177,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
@@ -1192,7 +1189,7 @@
         <v>38</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
@@ -1204,7 +1201,7 @@
         <v>39</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
@@ -1216,7 +1213,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
@@ -1228,7 +1225,7 @@
         <v>41</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
@@ -1240,7 +1237,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
@@ -1252,7 +1249,7 @@
         <v>43</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
@@ -1264,7 +1261,7 @@
         <v>44</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
@@ -1277,7 +1274,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>120</v>
+        <v>203</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>